<commit_message>
finito GF31 i BCH
</commit_message>
<xml_diff>
--- a/TestsGF31.xlsx
+++ b/TestsGF31.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michal/IT/PWr/NIDUC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19E5A73-15AC-F647-8757-A470293EAF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC1E13A-84E8-6844-83B3-06B8B10936F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="620" windowWidth="28040" windowHeight="16100" xr2:uid="{80C9E6B0-AF67-704E-9512-A3204CBA9E52}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>OK</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>dlaczego przy dwóch X udaje mu się skorygować</t>
+  </si>
+  <si>
+    <t>(Tak się liczby dobrały, że jakoś udało mu się skorygować, ale źle)</t>
   </si>
 </sst>
 </file>
@@ -137,11 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +483,7 @@
   <dimension ref="B1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,17 +545,18 @@
       <c r="G4" t="s">
         <v>9</v>
       </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="D5">
-        <v>482</v>
-      </c>
-      <c r="F5" s="2">
-        <v>518</v>
-      </c>
+      <c r="D5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F5" s="4"/>
       <c r="G5" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
update gf31 tests result
</commit_message>
<xml_diff>
--- a/TestsGF31.xlsx
+++ b/TestsGF31.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michal/IT/PWr/NIDUC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9200A14-8B33-774D-BAD5-395F1149B8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9895D016-8BF7-A44A-883C-E97E4B8F5467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="620" windowWidth="28040" windowHeight="16100" xr2:uid="{80C9E6B0-AF67-704E-9512-A3204CBA9E52}"/>
   </bookViews>
@@ -122,12 +122,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -136,9 +151,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,7 +491,7 @@
   <dimension ref="B1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B1" sqref="B1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,104 +502,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>1000</v>
       </c>
-      <c r="G2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="C3" s="1"/>
+      <c r="D3" s="2">
         <v>1000</v>
       </c>
-      <c r="G3" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="3">
         <v>132</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>868</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1">
+      <c r="C5" s="1"/>
+      <c r="D5" s="2">
         <v>1000</v>
       </c>
-      <c r="G5" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="2">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="3">
         <v>16</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>984</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="1">
+      <c r="C7" s="1"/>
+      <c r="D7" s="2">
         <v>11</v>
       </c>
-      <c r="F7" s="1">
+      <c r="E7" s="1"/>
+      <c r="F7" s="2">
         <v>989</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>